<commit_message>
stm2017 création du loop
</commit_message>
<xml_diff>
--- a/hepvs_2020_lm/hepvs2020_lm_raw.xlsx
+++ b/hepvs_2020_lm/hepvs2020_lm_raw.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolasbressoud/Documents/GitHub/r-projects/hepvs_2020_lm/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE5D71FF-B226-AC43-A3A3-1AF97FD9BDD9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56DFF8EC-A3AB-6A48-8FC0-F21ADB0FC678}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19160" windowHeight="21600" xr2:uid="{A293DA52-7156-C54C-BCD7-F8A433473A5C}"/>
+    <workbookView xWindow="9920" yWindow="980" windowWidth="19160" windowHeight="19520" xr2:uid="{A293DA52-7156-C54C-BCD7-F8A433473A5C}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -156,7 +156,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -168,6 +168,13 @@
       <u/>
       <sz val="12"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -194,9 +201,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -514,8 +522,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A578A9C3-64F0-BD46-B45E-885F700BE51E}">
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="224" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" zoomScale="224" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -669,10 +677,10 @@
       <c r="B6" t="s">
         <v>0</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="2" t="s">
         <v>32</v>
       </c>
       <c r="F6" s="1" t="s">

</xml_diff>